<commit_message>
Module 2 (Water) coupled
</commit_message>
<xml_diff>
--- a/condiciones_iniciales/parameters.xlsx
+++ b/condiciones_iniciales/parameters.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.amador\Desktop\simulador-resiliencia\herramienta-resiliencia-simulador\condiciones_iniciales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FD38A2-4EA2-4DDF-9F6D-79873B9323AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92839E5-F7DF-429F-855F-D135AE48FD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transformation_rates (2)" sheetId="2" r:id="rId1"/>
     <sheet name="transformation_rates" sheetId="1" r:id="rId2"/>
+    <sheet name="initial_conditions" sheetId="3" r:id="rId3"/>
+    <sheet name="water_parameters" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="94">
   <si>
     <t>'Agropecuario heterogeneo'</t>
   </si>
@@ -70,13 +72,259 @@
   </si>
   <si>
     <t>matriz</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Vaa</t>
+  </si>
+  <si>
+    <t>AdC</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Volumen de agua almacenado</t>
+  </si>
+  <si>
+    <t>Agua disponible para consumo</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Tasa</t>
+  </si>
+  <si>
+    <t>Precipitación</t>
+  </si>
+  <si>
+    <t>tprpm</t>
+  </si>
+  <si>
+    <t>fac</t>
+  </si>
+  <si>
+    <t>Factor de conversión (mm a m^^3)</t>
+  </si>
+  <si>
+    <t>Fpera_min</t>
+  </si>
+  <si>
+    <t>EaOc</t>
+  </si>
+  <si>
+    <t>Entradas de otras cuencas</t>
+  </si>
+  <si>
+    <t>Factor de perdidas</t>
+  </si>
+  <si>
+    <t>tsaoc_min</t>
+  </si>
+  <si>
+    <t>tretCob1</t>
+  </si>
+  <si>
+    <t>tretCob2</t>
+  </si>
+  <si>
+    <t>tretCob3</t>
+  </si>
+  <si>
+    <t>tretCob4</t>
+  </si>
+  <si>
+    <t>tretCob5</t>
+  </si>
+  <si>
+    <t>tretCob6</t>
+  </si>
+  <si>
+    <t>tretCob7</t>
+  </si>
+  <si>
+    <t>tretCob8</t>
+  </si>
+  <si>
+    <t>tretCob9</t>
+  </si>
+  <si>
+    <t>tretCob10</t>
+  </si>
+  <si>
+    <t>tretCob11</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 1</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 2</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 3</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 4</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 5</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 6</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 7</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 8</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 9</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 10</t>
+  </si>
+  <si>
+    <t>Capacidad de retención de la cobertura 11</t>
+  </si>
+  <si>
+    <t>Tasa de salida hacia otras cuencas</t>
+  </si>
+  <si>
+    <t>pac</t>
+  </si>
+  <si>
+    <t>tpca</t>
+  </si>
+  <si>
+    <t>tasa promedio de consumo de agua</t>
+  </si>
+  <si>
+    <t>Porcentaje de agua que va hacia otras cuencas usada para consumo</t>
+  </si>
+  <si>
+    <t>Consumo 1</t>
+  </si>
+  <si>
+    <t>Consumo 2</t>
+  </si>
+  <si>
+    <t>Consumo 3</t>
+  </si>
+  <si>
+    <t>Consumo 4</t>
+  </si>
+  <si>
+    <t>Consumo 5</t>
+  </si>
+  <si>
+    <t>Consumo 6</t>
+  </si>
+  <si>
+    <t>Consumo 7</t>
+  </si>
+  <si>
+    <t>Consumo 8</t>
+  </si>
+  <si>
+    <t>Consumo de agua por actividad 1</t>
+  </si>
+  <si>
+    <t>Consumo de agua por actividad 2</t>
+  </si>
+  <si>
+    <t>Consumo de agua por actividad 3</t>
+  </si>
+  <si>
+    <t>Consumo de agua por actividad 5</t>
+  </si>
+  <si>
+    <t>Consumo de agua por actividad 4</t>
+  </si>
+  <si>
+    <t>Consumo de agua por actividad 7</t>
+  </si>
+  <si>
+    <t>Consumo de agua por actividad 6</t>
+  </si>
+  <si>
+    <t>Consumo de agua por actividad 8</t>
+  </si>
+  <si>
+    <t>Iact1</t>
+  </si>
+  <si>
+    <t>Iact2</t>
+  </si>
+  <si>
+    <t>Iact3</t>
+  </si>
+  <si>
+    <t>Iact4</t>
+  </si>
+  <si>
+    <t>Iact5</t>
+  </si>
+  <si>
+    <t>Iact6</t>
+  </si>
+  <si>
+    <t>Iact7</t>
+  </si>
+  <si>
+    <t>Iact8</t>
+  </si>
+  <si>
+    <t>Iact9</t>
+  </si>
+  <si>
+    <t>Iact10</t>
+  </si>
+  <si>
+    <t>Iact11</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 1</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 2</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 3</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 5</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 4</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 6</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 7</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 8</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 9</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 10</t>
+  </si>
+  <si>
+    <t>Intensidad de la afectación de la calidad de agua por la actividad 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,16 +332,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -241,11 +517,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -274,6 +604,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +896,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L12"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,43 +960,43 @@
       </c>
       <c r="C2" s="3">
         <f ca="1">0.005+RAND()*(0.01-0.005)</f>
-        <v>7.7654604797867122E-3</v>
+        <v>5.014847877929161E-3</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="C2:L12" ca="1" si="0">0.005+RAND()*(0.01-0.005)</f>
-        <v>9.1754168889256766E-3</v>
+        <v>5.5625192943626204E-3</v>
       </c>
       <c r="E2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4565321429019916E-3</v>
+        <v>8.1783060438075112E-3</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0322495460982265E-3</v>
+        <v>8.0090637598496852E-3</v>
       </c>
       <c r="G2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.516127237213799E-3</v>
+        <v>9.8374834067567595E-3</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6270423763765728E-3</v>
+        <v>6.7282421000824707E-3</v>
       </c>
       <c r="I2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8319958784825381E-3</v>
+        <v>7.9591169658645121E-3</v>
       </c>
       <c r="J2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9362010811813138E-3</v>
+        <v>7.5262388628383487E-3</v>
       </c>
       <c r="K2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4518150177586041E-3</v>
+        <v>5.1648163506376847E-3</v>
       </c>
       <c r="L2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5640796939454251E-3</v>
+        <v>9.8985530355227835E-3</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -666,46 +1005,46 @@
       </c>
       <c r="B3" s="3">
         <f t="shared" ref="B3:B11" ca="1" si="1">0.005+RAND()*(0.01-0.005)</f>
-        <v>7.0394157200762732E-3</v>
+        <v>8.0500868518326493E-3</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.1163887497986221E-3</v>
+        <v>7.9070560562156441E-3</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9605200225593654E-3</v>
+        <v>6.919750473659554E-3</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.975884154524937E-3</v>
+        <v>7.4324297320421152E-3</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8035188669190762E-3</v>
+        <v>7.5892492931960214E-3</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8765902460152197E-3</v>
+        <v>6.5808410470306949E-3</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.2222397196235154E-3</v>
+        <v>7.6503157280541686E-3</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8407325742118894E-3</v>
+        <v>6.730769942728948E-3</v>
       </c>
       <c r="K3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.971328032851584E-3</v>
+        <v>7.3431360957414218E-3</v>
       </c>
       <c r="L3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1275143797897436E-3</v>
+        <v>8.7328643413033032E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -714,46 +1053,46 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8.28203860943523E-3</v>
+        <v>6.4025815796537782E-3</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6135882538632483E-3</v>
+        <v>8.384862358616612E-3</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8965862221637385E-3</v>
+        <v>8.9438843628628951E-3</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3056623159403625E-3</v>
+        <v>6.2899009932211895E-3</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5160328837094977E-3</v>
+        <v>6.9265928006180082E-3</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.785488220816204E-3</v>
+        <v>7.1845382405560272E-3</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8682713013119629E-3</v>
+        <v>5.9285368855721407E-3</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1910874565895028E-3</v>
+        <v>7.5744801875692706E-3</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4039007806078524E-3</v>
+        <v>5.5651703684874059E-3</v>
       </c>
       <c r="L4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7540311824594675E-3</v>
+        <v>8.4117216331851888E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -762,46 +1101,46 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3051076576800076E-3</v>
+        <v>6.4321837085188826E-3</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.358031090007649E-3</v>
+        <v>9.8231281674439688E-3</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8859118854206003E-3</v>
+        <v>9.4055153523828847E-3</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9621990654632613E-3</v>
+        <v>5.1779970163905766E-3</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2657084689410666E-3</v>
+        <v>9.4455984540651461E-3</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0607430824957372E-3</v>
+        <v>8.2070306467292437E-3</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.983776609284083E-3</v>
+        <v>7.095134912093082E-3</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.507890484283593E-3</v>
+        <v>9.8623004423339898E-3</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2847472580256393E-3</v>
+        <v>7.4843055315946729E-3</v>
       </c>
       <c r="L5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3101148021169583E-3</v>
+        <v>9.5843870042088344E-3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -810,46 +1149,46 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7815769317756785E-3</v>
+        <v>6.1661757434146383E-3</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0248843910013601E-3</v>
+        <v>5.1497697446355687E-3</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6286780027535967E-3</v>
+        <v>7.3554786241019163E-3</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1475578747137282E-3</v>
+        <v>9.9387565899715941E-3</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3979536399218201E-3</v>
+        <v>6.0966370680278128E-3</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1504568913697839E-3</v>
+        <v>5.8684640347058201E-3</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.253777915178691E-3</v>
+        <v>9.6531715010734521E-3</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1264960294527019E-3</v>
+        <v>9.3399875996047592E-3</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4559965210405279E-3</v>
+        <v>6.6530524814150576E-3</v>
       </c>
       <c r="L6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0815759448536941E-3</v>
+        <v>8.7967670461278069E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -858,46 +1197,46 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7415606998127596E-3</v>
+        <v>6.1453014991815786E-3</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.5599929024249219E-3</v>
+        <v>5.5799495474154002E-3</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7263815553313192E-3</v>
+        <v>7.1035277518755723E-3</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7120199518381072E-3</v>
+        <v>9.0370417845742311E-3</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.104809313739904E-3</v>
+        <v>6.2089579696535642E-3</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9416860435828924E-3</v>
+        <v>6.2580976949202808E-3</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1786506965290245E-3</v>
+        <v>5.8107765345705165E-3</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8898288044930223E-3</v>
+        <v>6.1522061824158779E-3</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8288054060310572E-3</v>
+        <v>7.5634867605845722E-3</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6073546737250776E-3</v>
+        <v>9.6220923430928151E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -906,46 +1245,46 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3245974396578271E-3</v>
+        <v>6.7411932204339223E-3</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9809936786593757E-3</v>
+        <v>6.7991704412570728E-3</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9608087010895273E-3</v>
+        <v>9.0971395854604377E-3</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9444092469160869E-3</v>
+        <v>5.3245453568982401E-3</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7389497773555438E-3</v>
+        <v>8.676664899235402E-3</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7694584746889963E-3</v>
+        <v>9.9500345267596029E-3</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9505964526562882E-3</v>
+        <v>6.1033989856349585E-3</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0140645566389385E-3</v>
+        <v>7.8187925695468227E-3</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4370758288982379E-3</v>
+        <v>7.4974808571569851E-3</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3633877817728339E-3</v>
+        <v>9.2194180561717687E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -954,46 +1293,46 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7372822688426077E-3</v>
+        <v>7.7459612556098536E-3</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6944388260996232E-3</v>
+        <v>9.1098587503877677E-3</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.361151798406359E-3</v>
+        <v>5.1362651954452773E-3</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9434361917738285E-3</v>
+        <v>7.1940565498486101E-3</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8094742219502371E-3</v>
+        <v>9.1928844706053343E-3</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7604163282530402E-3</v>
+        <v>5.2206444453780643E-3</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5746255599053129E-3</v>
+        <v>6.4122045813693853E-3</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7954109868502231E-3</v>
+        <v>6.9716983011587821E-3</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.024101851558797E-3</v>
+        <v>5.7395776067915485E-3</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9089075468994534E-3</v>
+        <v>9.5184988016269768E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1002,46 +1341,46 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0622094881271765E-3</v>
+        <v>7.3212681264326097E-3</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7997666135701805E-3</v>
+        <v>8.7359405193153522E-3</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3210007465038485E-3</v>
+        <v>9.1955436077576919E-3</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8064708860062174E-3</v>
+        <v>9.9929422705960606E-3</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4191627778483265E-3</v>
+        <v>7.1261313469246652E-3</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8375159211425699E-3</v>
+        <v>6.8654694309746222E-3</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8650309470744426E-3</v>
+        <v>5.2656037900683534E-3</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3814027940553237E-3</v>
+        <v>8.1261033531213125E-3</v>
       </c>
       <c r="J10" s="2">
         <v>0</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4784253262012972E-3</v>
+        <v>9.5875762213157474E-3</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1196709201278088E-3</v>
+        <v>8.4398016856910181E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1050,46 +1389,46 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1495418153846823E-3</v>
+        <v>7.1741338851236142E-3</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8383552194410868E-3</v>
+        <v>6.3532638260476084E-3</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.034800676083839E-3</v>
+        <v>9.2006656646846756E-3</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1103438872592243E-3</v>
+        <v>6.906438876394143E-3</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4243971618722727E-3</v>
+        <v>7.0775878618679275E-3</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3143962116363793E-3</v>
+        <v>9.028406347312494E-3</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0406491705637319E-3</v>
+        <v>9.4794151093843832E-3</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.1023762879121339E-3</v>
+        <v>5.6546863764879675E-3</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5439425125018809E-3</v>
+        <v>6.8204682623438893E-3</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5349040800271024E-3</v>
+        <v>5.5352298069056604E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1098,43 +1437,43 @@
       </c>
       <c r="B12" s="3">
         <f ca="1">0.005+RAND()*(0.01-0.005)</f>
-        <v>8.0507927183057458E-3</v>
+        <v>6.7671088813684071E-3</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.763876596906521E-3</v>
+        <v>5.6274871861313139E-3</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3155209570248099E-3</v>
+        <v>6.8464784766321023E-3</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0922042613259317E-3</v>
+        <v>9.4175028574461448E-3</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7047563337709884E-3</v>
+        <v>5.1102006179383772E-3</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5009383908133239E-3</v>
+        <v>8.7741898790453E-3</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0883206294264384E-3</v>
+        <v>7.4834966470085579E-3</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7347488959594764E-3</v>
+        <v>6.5261577365649179E-3</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.754966764074187E-3</v>
+        <v>8.509604435473897E-3</v>
       </c>
       <c r="K12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7821698598599301E-3</v>
+        <v>8.9401932680435309E-3</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
@@ -1161,7 +1500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1652,4 +1991,497 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5317EF6B-5B69-4FC9-A4C0-27E0A6079B57}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>500000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>50000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55838E95-87B8-4785-BD8F-7353E52C3BF4}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="61" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="18">
+        <v>8</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="18">
+        <v>100</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="18">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0.21</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.18</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0.23</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>0.2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>15000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
+        <v>20000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>30000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23">
+        <v>50000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24">
+        <v>12000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25">
+        <v>4200</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26">
+        <v>12000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27">
+        <v>7000</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modules 3, 4 y 5 updated
</commit_message>
<xml_diff>
--- a/condiciones_iniciales/parameters.xlsx
+++ b/condiciones_iniciales/parameters.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.amador\Desktop\simulador-resiliencia\herramienta-resiliencia-simulador\condiciones_iniciales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92839E5-F7DF-429F-855F-D135AE48FD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E6F997-E463-4138-8F40-E9A86EF8A0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transformation_rates (2)" sheetId="2" r:id="rId1"/>
     <sheet name="transformation_rates" sheetId="1" r:id="rId2"/>
     <sheet name="initial_conditions" sheetId="3" r:id="rId3"/>
     <sheet name="water_parameters" sheetId="4" r:id="rId4"/>
+    <sheet name="Abiotic_Variables" sheetId="5" r:id="rId5"/>
+    <sheet name="Habitat_Availability" sheetId="6" r:id="rId6"/>
+    <sheet name="Functional_diversity" sheetId="7" r:id="rId7"/>
+    <sheet name="Diversity_of_activities" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="166">
   <si>
     <t>'Agropecuario heterogeneo'</t>
   </si>
@@ -318,6 +323,222 @@
   </si>
   <si>
     <t>Intensidad de la afectación de la calidad de agua por la actividad 11</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>DpohaEs_1max</t>
+  </si>
+  <si>
+    <t>DpohaEs_2max</t>
+  </si>
+  <si>
+    <t>DpohaEs_3max</t>
+  </si>
+  <si>
+    <t>DpohaEs_4max</t>
+  </si>
+  <si>
+    <t>DpohaEs_5max</t>
+  </si>
+  <si>
+    <t>DpohaEs_6max</t>
+  </si>
+  <si>
+    <t>DpohaEs_7max</t>
+  </si>
+  <si>
+    <t>DpohaEs_8max</t>
+  </si>
+  <si>
+    <t>DpohaEs_9max</t>
+  </si>
+  <si>
+    <t>DpohaEs_10max</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 1</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 2</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 3</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 4</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 5</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 6</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 7</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 8</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 9</t>
+  </si>
+  <si>
+    <t>Distrribución potencial de hábitat especie 10</t>
+  </si>
+  <si>
+    <t>UES1</t>
+  </si>
+  <si>
+    <t>UES2</t>
+  </si>
+  <si>
+    <t>UES3</t>
+  </si>
+  <si>
+    <t>UES4</t>
+  </si>
+  <si>
+    <t>UES5</t>
+  </si>
+  <si>
+    <t>UES6</t>
+  </si>
+  <si>
+    <t>UES7</t>
+  </si>
+  <si>
+    <t>UES8</t>
+  </si>
+  <si>
+    <t>UES9</t>
+  </si>
+  <si>
+    <t>UES10</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 1</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 2</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 3</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 4</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 5</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 6</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 7</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 8</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 9</t>
+  </si>
+  <si>
+    <t>Umbral de desaparición de la especie 10</t>
+  </si>
+  <si>
+    <t>Función 1</t>
+  </si>
+  <si>
+    <t>Función 2</t>
+  </si>
+  <si>
+    <t>Función 3</t>
+  </si>
+  <si>
+    <t>Función 4</t>
+  </si>
+  <si>
+    <t>Función 5</t>
+  </si>
+  <si>
+    <t>Función 6</t>
+  </si>
+  <si>
+    <t>Función 7</t>
+  </si>
+  <si>
+    <t>Función 8</t>
+  </si>
+  <si>
+    <t>Función 9</t>
+  </si>
+  <si>
+    <t>Función 10</t>
+  </si>
+  <si>
+    <t>Especie 1</t>
+  </si>
+  <si>
+    <t>Especie 2</t>
+  </si>
+  <si>
+    <t>Especie 3</t>
+  </si>
+  <si>
+    <t>Especie 4</t>
+  </si>
+  <si>
+    <t>Especie 5</t>
+  </si>
+  <si>
+    <t>Especie 6</t>
+  </si>
+  <si>
+    <t>Especie 7</t>
+  </si>
+  <si>
+    <t>Especie 8</t>
+  </si>
+  <si>
+    <t>Especie 9</t>
+  </si>
+  <si>
+    <t>Especie 10</t>
+  </si>
+  <si>
+    <t>Pasturas homogeneas'</t>
+  </si>
+  <si>
+    <t>PAE</t>
+  </si>
+  <si>
+    <t>Población en el área de estudio</t>
+  </si>
+  <si>
+    <t>tPMig</t>
+  </si>
+  <si>
+    <t>Tasa de mogración</t>
+  </si>
+  <si>
+    <t>tINPAE</t>
+  </si>
+  <si>
+    <t>Tasa de incremento neto de población</t>
+  </si>
+  <si>
+    <t>tDFPAE</t>
+  </si>
+  <si>
+    <t>Tasa de desplazamiento forzado</t>
+  </si>
+  <si>
+    <t>tEMig</t>
+  </si>
+  <si>
+    <t>Tasa de emigración</t>
   </si>
 </sst>
 </file>
@@ -575,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -613,6 +834,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,7 +1120,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,44 +1183,44 @@
         <v>0</v>
       </c>
       <c r="C2" s="3">
-        <f ca="1">0.005+RAND()*(0.01-0.005)</f>
-        <v>5.014847877929161E-3</v>
+        <f ca="1">0.01+RAND()*(0.2-0.01)</f>
+        <v>7.9173580586418574E-2</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="C2:L12" ca="1" si="0">0.005+RAND()*(0.01-0.005)</f>
-        <v>5.5625192943626204E-3</v>
+        <f t="shared" ref="D2:L11" ca="1" si="0">0.01+RAND()*(0.2-0.01)</f>
+        <v>7.8351891616017882E-2</v>
       </c>
       <c r="E2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1783060438075112E-3</v>
+        <v>0.15963777962076331</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.0090637598496852E-3</v>
+        <v>0.19323694741583838</v>
       </c>
       <c r="G2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8374834067567595E-3</v>
+        <v>0.12725547278941518</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7282421000824707E-3</v>
+        <v>8.5246308018340905E-2</v>
       </c>
       <c r="I2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.9591169658645121E-3</v>
+        <v>0.16486278575302041</v>
       </c>
       <c r="J2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5262388628383487E-3</v>
+        <v>0.15938641296411635</v>
       </c>
       <c r="K2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1648163506376847E-3</v>
+        <v>0.13620435602175757</v>
       </c>
       <c r="L2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8985530355227835E-3</v>
+        <v>0.11591198388378585</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1005,46 +1229,46 @@
       </c>
       <c r="B3" s="3">
         <f t="shared" ref="B3:B11" ca="1" si="1">0.005+RAND()*(0.01-0.005)</f>
-        <v>8.0500868518326493E-3</v>
+        <v>8.0085333240221528E-3</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.9070560562156441E-3</v>
+        <f t="shared" ref="C3:K12" ca="1" si="2">0.005+RAND()*(0.01-0.005)</f>
+        <v>8.9448099986898268E-3</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.919750473659554E-3</v>
+        <v>0.19330204135644213</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4324297320421152E-3</v>
+        <v>0.19586128357029334</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5892492931960214E-3</v>
+        <v>9.4204537228907786E-2</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5808410470306949E-3</v>
+        <v>0.10584899537195018</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6503157280541686E-3</v>
+        <v>0.11528996300681207</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.730769942728948E-3</v>
+        <v>0.12263164107421723</v>
       </c>
       <c r="K3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3431360957414218E-3</v>
+        <v>1.5842432428387881E-2</v>
       </c>
       <c r="L3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7328643413033032E-3</v>
+        <v>3.830634853691002E-2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1053,46 +1277,46 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4025815796537782E-3</v>
+        <v>9.4397348994932004E-3</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.384862358616612E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.3984401653494564E-3</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9438843628628951E-3</v>
+        <v>0.17954909634175095</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2899009932211895E-3</v>
+        <v>0.1018211334632355</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9265928006180082E-3</v>
+        <v>0.13045239063412417</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1845382405560272E-3</v>
+        <v>0.17353621532690749</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9285368855721407E-3</v>
+        <v>3.6469802284661845E-2</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5744801875692706E-3</v>
+        <v>9.7300984244303376E-2</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5651703684874059E-3</v>
+        <v>7.1888006873114502E-2</v>
       </c>
       <c r="L4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4117216331851888E-3</v>
+        <v>0.18387208403763286</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1101,46 +1325,46 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4321837085188826E-3</v>
+        <v>8.9879690467116261E-3</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.8231281674439688E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1696220744962707E-3</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.4055153523828847E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.0936231147127014E-3</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1779970163905766E-3</v>
+        <v>8.9935223640780451E-2</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4455984540651461E-3</v>
+        <v>5.5209304776175229E-2</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2070306467292437E-3</v>
+        <v>6.7848656276408015E-2</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.095134912093082E-3</v>
+        <v>0.15685118911229498</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8623004423339898E-3</v>
+        <v>0.18174239595554548</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4843055315946729E-3</v>
+        <v>0.14954757805207949</v>
       </c>
       <c r="L5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5843870042088344E-3</v>
+        <v>3.5357146774095329E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1149,46 +1373,46 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1661757434146383E-3</v>
+        <v>5.6550371982495009E-3</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1497697446355687E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.8770767977627242E-3</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.3554786241019163E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.9004737348243488E-3</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.9387565899715941E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.0247261421129467E-3</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0966370680278128E-3</v>
+        <v>0.1773228386515418</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8684640347058201E-3</v>
+        <v>2.0524725240281812E-2</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6531715010734521E-3</v>
+        <v>0.16710936495561432</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3399875996047592E-3</v>
+        <v>8.5531423908213347E-2</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6530524814150576E-3</v>
+        <v>0.19369679431949116</v>
       </c>
       <c r="L6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7967670461278069E-3</v>
+        <v>5.6628360372919594E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1197,46 +1421,46 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1453014991815786E-3</v>
+        <v>7.3338915578194802E-3</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.5799495474154002E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.2072304586958437E-3</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.1035277518755723E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.9073396291643952E-3</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.0370417845742311E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.6049692061355318E-3</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.2089579696535642E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.212626687681337E-3</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2580976949202808E-3</v>
+        <v>3.5989861668289026E-2</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8107765345705165E-3</v>
+        <v>0.10171744388909248</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1522061824158779E-3</v>
+        <v>1.0553954845000218E-2</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5634867605845722E-3</v>
+        <v>7.1070157297466421E-2</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6220923430928151E-3</v>
+        <v>0.12442399362477746</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -1245,46 +1469,46 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7411932204339223E-3</v>
+        <v>8.4265885163788204E-3</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.7991704412570728E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.5232532923320333E-3</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.0971395854604377E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4444894207536735E-3</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3245453568982401E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.0974978160014352E-3</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.676664899235402E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.8751028919247199E-3</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.9500345267596029E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.0627827969183717E-3</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1033989856349585E-3</v>
+        <v>0.13705183580118052</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8187925695468227E-3</v>
+        <v>2.7870742204139626E-2</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4974808571569851E-3</v>
+        <v>9.0455116003040223E-2</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2194180561717687E-3</v>
+        <v>9.0835809348245269E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1293,46 +1517,46 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7459612556098536E-3</v>
+        <v>6.5068074635077407E-3</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.1098587503877677E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.6930963562983537E-3</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1362651954452773E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4911661413094265E-3</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.1940565498486101E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.2810581583166922E-3</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.1928844706053343E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.5850593265446966E-3</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2206444453780643E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.5031808615995148E-3</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.4122045813693853E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.157272111699209E-3</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9716983011587821E-3</v>
+        <v>0.16806548544333177</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7395776067915485E-3</v>
+        <v>3.2176705636919004E-2</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5184988016269768E-3</v>
+        <v>7.7123874582905386E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1341,46 +1565,46 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3212681264326097E-3</v>
+        <v>6.7696326870713888E-3</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.7359405193153522E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.0815321971706676E-3</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.1955436077576919E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0615145353980137E-3</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.9929422705960606E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.1588928224346864E-3</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.1261313469246652E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.5689452202377297E-3</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.8654694309746222E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.3730341484126204E-3</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2656037900683534E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.4357011398241899E-3</v>
       </c>
       <c r="I10" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.1261033531213125E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.3555861023807175E-3</v>
       </c>
       <c r="J10" s="2">
         <v>0</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5875762213157474E-3</v>
+        <v>2.6044351657805158E-2</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4398016856910181E-3</v>
+        <v>0.15395771367464584</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1389,46 +1613,46 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1741338851236142E-3</v>
+        <v>8.2890420996925285E-3</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.3532638260476084E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.7930143792003318E-3</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.2006656646846756E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.1316640184822923E-3</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.906438876394143E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.4462146614988987E-3</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.0775878618679275E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.6573543764302297E-3</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.028406347312494E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.7338052534083359E-3</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.4794151093843832E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.1658238638394236E-3</v>
       </c>
       <c r="I11" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.6546863764879675E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.3520844415033175E-3</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.8204682623438893E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.7815067599480659E-3</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5352298069056604E-3</v>
+        <v>0.1472561303858545</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1437,43 +1661,43 @@
       </c>
       <c r="B12" s="3">
         <f ca="1">0.005+RAND()*(0.01-0.005)</f>
-        <v>6.7671088813684071E-3</v>
+        <v>7.7535628716342972E-3</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.6274871861313139E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.1033493709502776E-3</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.8464784766321023E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.395040785202164E-3</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.4175028574461448E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.2129887885004247E-3</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1102006179383772E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.1762853869722608E-3</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.7741898790453E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.7952822965719621E-3</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.4834966470085579E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.1449093778684462E-3</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.5261577365649179E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.486607500102705E-3</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.509604435473897E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4446801188258662E-3</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.9401932680435309E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4418976067120914E-3</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
@@ -1498,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,8 +1763,8 @@
       <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>5</v>
+      <c r="G1" s="21" t="s">
+        <v>155</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>6</v>
@@ -1566,34 +1790,34 @@
         <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>8.4944290196175554E-3</v>
+        <v>0.19573281797254957</v>
       </c>
       <c r="D2" s="3">
-        <v>6.8947164960883982E-3</v>
+        <v>0.1</v>
       </c>
       <c r="E2" s="3">
-        <v>6.3238098474513085E-3</v>
+        <v>2.154252864320012E-2</v>
       </c>
       <c r="F2" s="3">
-        <v>5.7116669401302339E-3</v>
+        <v>0.17191792379311063</v>
       </c>
       <c r="G2" s="3">
-        <v>8.8976090065293074E-3</v>
+        <v>0.18873336486953565</v>
       </c>
       <c r="H2" s="3">
-        <v>7.6942134732131042E-3</v>
+        <v>0.1181826814912897</v>
       </c>
       <c r="I2" s="3">
-        <v>7.9641135263243922E-3</v>
+        <v>1.3117965817845988E-2</v>
       </c>
       <c r="J2" s="3">
-        <v>8.7599432229652913E-3</v>
+        <v>6.9073329665386596E-2</v>
       </c>
       <c r="K2" s="3">
-        <v>6.0180431500872029E-3</v>
+        <v>6.4260819768181557E-2</v>
       </c>
       <c r="L2" s="3">
-        <v>5.9160158367827171E-3</v>
+        <v>8.2770035633121505E-2</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1601,37 +1825,37 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>7.8948016019962652E-3</v>
+        <v>6.0720934624794139E-3</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>5.9638187525565848E-3</v>
+        <v>8.4727711486920158E-3</v>
       </c>
       <c r="E3" s="3">
-        <v>5.8773065224417779E-3</v>
+        <v>0.18292622763176522</v>
       </c>
       <c r="F3" s="3">
-        <v>9.6640198832164438E-3</v>
+        <v>9.3633523240937572E-2</v>
       </c>
       <c r="G3" s="3">
-        <v>6.7830544779763852E-3</v>
+        <v>0.17739963998277414</v>
       </c>
       <c r="H3" s="3">
-        <v>9.9738305597310683E-3</v>
+        <v>6.2686886149702331E-2</v>
       </c>
       <c r="I3" s="3">
-        <v>5.5519574382861788E-3</v>
+        <v>6.3385076099946591E-2</v>
       </c>
       <c r="J3" s="3">
-        <v>5.4697384742804396E-3</v>
+        <v>0.19418611080215736</v>
       </c>
       <c r="K3" s="3">
-        <v>6.1004806556023364E-3</v>
+        <v>0.14670009020309244</v>
       </c>
       <c r="L3" s="3">
-        <v>6.2170925413482141E-3</v>
+        <v>0.15346990892753165</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1639,37 +1863,37 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>6.1436106263326115E-3</v>
+        <v>8.4173623415741312E-3</v>
       </c>
       <c r="C4" s="3">
-        <v>8.4423648699886427E-3</v>
+        <v>8.5928233806717991E-3</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>9.9951681567270328E-3</v>
+        <v>0.19515411227672835</v>
       </c>
       <c r="F4" s="3">
-        <v>7.4269949290302669E-3</v>
+        <v>7.2327418390243689E-2</v>
       </c>
       <c r="G4" s="3">
-        <v>7.1986044134858575E-3</v>
+        <v>6.350213726355794E-2</v>
       </c>
       <c r="H4" s="3">
-        <v>6.6172117948311814E-3</v>
+        <v>0.16452215588825372</v>
       </c>
       <c r="I4" s="3">
-        <v>7.8073898873504254E-3</v>
+        <v>0.10503539287988439</v>
       </c>
       <c r="J4" s="3">
-        <v>6.7906344072040849E-3</v>
+        <v>0.16690253290072471</v>
       </c>
       <c r="K4" s="3">
-        <v>9.0687608255000558E-3</v>
+        <v>0.17429880406647416</v>
       </c>
       <c r="L4" s="3">
-        <v>8.7387296885653633E-3</v>
+        <v>0.11800019429273578</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1677,37 +1901,37 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>6.7341381873334072E-3</v>
+        <v>6.2101378711803927E-3</v>
       </c>
       <c r="C5" s="3">
-        <v>5.9261000479068696E-3</v>
+        <v>6.6396451468447521E-3</v>
       </c>
       <c r="D5" s="3">
-        <v>8.9770954769286624E-3</v>
+        <v>9.7591087042133255E-3</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="3">
-        <v>8.9927800301345395E-3</v>
+        <v>6.2382289698040744E-2</v>
       </c>
       <c r="G5" s="3">
-        <v>8.1828731471147408E-3</v>
+        <v>0.11689215492790632</v>
       </c>
       <c r="H5" s="3">
-        <v>8.6951420183647606E-3</v>
+        <v>1.7605170521890076E-2</v>
       </c>
       <c r="I5" s="3">
-        <v>5.3824587039153163E-3</v>
+        <v>4.0263263177040272E-2</v>
       </c>
       <c r="J5" s="3">
-        <v>7.7997465995245114E-3</v>
+        <v>7.7046825943686018E-2</v>
       </c>
       <c r="K5" s="3">
-        <v>7.8031193351873092E-3</v>
+        <v>3.0462012086750277E-2</v>
       </c>
       <c r="L5" s="3">
-        <v>7.2344151412589925E-3</v>
+        <v>0.14679107586545281</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1715,37 +1939,37 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>9.0759129270696973E-3</v>
+        <v>8.6470620736513078E-3</v>
       </c>
       <c r="C6" s="3">
-        <v>7.3225873784545197E-3</v>
+        <v>8.858885249166875E-3</v>
       </c>
       <c r="D6" s="3">
-        <v>5.563424929535204E-3</v>
+        <v>9.9128329457706665E-3</v>
       </c>
       <c r="E6" s="3">
-        <v>7.8623593128431604E-3</v>
+        <v>6.0858069181180408E-3</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
       </c>
       <c r="G6" s="3">
-        <v>8.6904382554554745E-3</v>
+        <v>0.1628558387896295</v>
       </c>
       <c r="H6" s="3">
-        <v>9.0547575768310101E-3</v>
+        <v>0.18813026709356898</v>
       </c>
       <c r="I6" s="3">
-        <v>8.0095819842944498E-3</v>
+        <v>5.77290599336178E-2</v>
       </c>
       <c r="J6" s="3">
-        <v>6.7247964631983216E-3</v>
+        <v>5.8233645703230037E-2</v>
       </c>
       <c r="K6" s="3">
-        <v>7.646759349275464E-3</v>
+        <v>3.5211138903162492E-2</v>
       </c>
       <c r="L6" s="3">
-        <v>8.6412113060728383E-3</v>
+        <v>0.18089931400353956</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1753,37 +1977,37 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>6.7380997776516297E-3</v>
+        <v>7.9866842205983113E-3</v>
       </c>
       <c r="C7" s="3">
-        <v>5.6074884043959237E-3</v>
+        <v>8.5394149156373111E-3</v>
       </c>
       <c r="D7" s="3">
-        <v>6.2832634400001742E-3</v>
+        <v>5.2824144291606333E-3</v>
       </c>
       <c r="E7" s="3">
-        <v>6.4373562223519502E-3</v>
+        <v>8.4866555835938148E-3</v>
       </c>
       <c r="F7" s="3">
-        <v>9.7988856038145784E-3</v>
+        <v>7.067064588302821E-3</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
       </c>
       <c r="H7" s="3">
-        <v>8.0435216216225187E-3</v>
+        <v>1.0953275414301317E-2</v>
       </c>
       <c r="I7" s="3">
-        <v>6.7599398061736942E-3</v>
+        <v>6.485047665891315E-2</v>
       </c>
       <c r="J7" s="3">
-        <v>5.3084223177913489E-3</v>
+        <v>6.9817566553436627E-2</v>
       </c>
       <c r="K7" s="3">
-        <v>9.9760117173850783E-3</v>
+        <v>0.12149912674754959</v>
       </c>
       <c r="L7" s="3">
-        <v>6.5458899756984899E-3</v>
+        <v>4.2359680483304726E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -1791,37 +2015,37 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>6.1283458200633318E-3</v>
+        <v>7.2203889979038319E-3</v>
       </c>
       <c r="C8" s="3">
-        <v>5.9044412835687855E-3</v>
+        <v>9.3022033308492839E-3</v>
       </c>
       <c r="D8" s="3">
-        <v>5.2462419485478189E-3</v>
+        <v>8.5633543760256156E-3</v>
       </c>
       <c r="E8" s="3">
-        <v>8.8133324104544709E-3</v>
+        <v>9.8427319279794593E-3</v>
       </c>
       <c r="F8" s="3">
-        <v>8.4725855998510138E-3</v>
+        <v>6.8067057505664585E-3</v>
       </c>
       <c r="G8" s="3">
-        <v>7.4633664857107103E-3</v>
+        <v>7.4446762347560409E-3</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="3">
-        <v>8.8045561427169527E-3</v>
+        <v>0.19747042317931204</v>
       </c>
       <c r="J8" s="3">
-        <v>9.1521142141311705E-3</v>
+        <v>2.8508846937610181E-2</v>
       </c>
       <c r="K8" s="3">
-        <v>7.3327634152953397E-3</v>
+        <v>0.16539708031621361</v>
       </c>
       <c r="L8" s="3">
-        <v>5.3080698782857752E-3</v>
+        <v>7.0438125717389152E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1829,37 +2053,37 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>7.5541340873660134E-3</v>
+        <v>8.7633350856316343E-3</v>
       </c>
       <c r="C9" s="3">
-        <v>9.1128248221592247E-3</v>
+        <v>8.2094536586940683E-3</v>
       </c>
       <c r="D9" s="3">
-        <v>9.7490359159332872E-3</v>
+        <v>9.3049316724396064E-3</v>
       </c>
       <c r="E9" s="3">
-        <v>7.7632132348352742E-3</v>
+        <v>7.1088983542616493E-3</v>
       </c>
       <c r="F9" s="3">
-        <v>5.0685986752992407E-3</v>
+        <v>5.2053298500599286E-3</v>
       </c>
       <c r="G9" s="3">
-        <v>7.7251853110738636E-3</v>
+        <v>5.362811993530581E-3</v>
       </c>
       <c r="H9" s="3">
-        <v>8.4793814918260515E-3</v>
+        <v>9.0188744345704765E-3</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
       </c>
       <c r="J9" s="3">
-        <v>6.3757100912638252E-3</v>
+        <v>1.0244344316160234E-2</v>
       </c>
       <c r="K9" s="3">
-        <v>9.1056520572820251E-3</v>
+        <v>0.12593844864280798</v>
       </c>
       <c r="L9" s="3">
-        <v>9.8373052707795214E-3</v>
+        <v>9.9999298542642445E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1867,37 +2091,37 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>9.6004790599766819E-3</v>
+        <v>7.7580356027287531E-3</v>
       </c>
       <c r="C10" s="3">
-        <v>5.0527644660918357E-3</v>
+        <v>5.4411059720114096E-3</v>
       </c>
       <c r="D10" s="3">
-        <v>6.5696377274664453E-3</v>
+        <v>5.1808991408880348E-3</v>
       </c>
       <c r="E10" s="3">
-        <v>7.3227969342866805E-3</v>
+        <v>6.9238204421003006E-3</v>
       </c>
       <c r="F10" s="3">
-        <v>6.5098896206596899E-3</v>
+        <v>8.1661300676200577E-3</v>
       </c>
       <c r="G10" s="3">
-        <v>9.8847418743596791E-3</v>
+        <v>6.4046163745725025E-3</v>
       </c>
       <c r="H10" s="3">
-        <v>9.596460170814846E-3</v>
+        <v>5.6732898952311277E-3</v>
       </c>
       <c r="I10" s="3">
-        <v>9.7503336060233928E-3</v>
+        <v>8.3769094446346105E-3</v>
       </c>
       <c r="J10" s="2">
         <v>0</v>
       </c>
       <c r="K10" s="3">
-        <v>5.4587507772416565E-3</v>
+        <v>0.18302474177095782</v>
       </c>
       <c r="L10" s="3">
-        <v>5.1891117703536452E-3</v>
+        <v>0.13426012421934161</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1905,37 +2129,37 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>8.1777083861465684E-3</v>
+        <v>5.8010220279186842E-3</v>
       </c>
       <c r="C11" s="3">
-        <v>5.3264195644582967E-3</v>
+        <v>7.7220530656772861E-3</v>
       </c>
       <c r="D11" s="3">
-        <v>6.777148815060802E-3</v>
+        <v>7.0407487969586366E-3</v>
       </c>
       <c r="E11" s="3">
-        <v>9.8692452301047569E-3</v>
+        <v>5.4877172551196221E-3</v>
       </c>
       <c r="F11" s="3">
-        <v>9.7961807824413667E-3</v>
+        <v>8.9898735686798591E-3</v>
       </c>
       <c r="G11" s="3">
-        <v>9.4480252251371039E-3</v>
+        <v>7.8961489287473242E-3</v>
       </c>
       <c r="H11" s="3">
-        <v>7.0550616041735511E-3</v>
+        <v>9.0968875015581298E-3</v>
       </c>
       <c r="I11" s="3">
-        <v>8.1626293088963107E-3</v>
+        <v>9.4999240301918801E-3</v>
       </c>
       <c r="J11" s="3">
-        <v>6.2156773208099456E-3</v>
+        <v>9.1386369123413747E-3</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
       <c r="L11" s="3">
-        <v>7.4048366632790191E-3</v>
+        <v>1.1865298297922263E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1943,41 +2167,1338 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>8.5212477620180971E-3</v>
+        <v>6.0029181952182932E-3</v>
       </c>
       <c r="C12" s="3">
-        <v>6.0047002705621126E-3</v>
+        <v>7.3174350541913135E-3</v>
       </c>
       <c r="D12" s="3">
-        <v>9.6418121796282893E-3</v>
+        <v>8.2330784633795426E-3</v>
       </c>
       <c r="E12" s="3">
-        <v>7.045794764094275E-3</v>
+        <v>9.3233722580055543E-3</v>
       </c>
       <c r="F12" s="3">
-        <v>6.9437022779515068E-3</v>
+        <v>5.703430551248034E-3</v>
       </c>
       <c r="G12" s="3">
-        <v>9.4473024331494411E-3</v>
+        <v>5.5303985261295659E-3</v>
       </c>
       <c r="H12" s="3">
-        <v>7.1893068304508031E-3</v>
+        <v>8.765545112282511E-3</v>
       </c>
       <c r="I12" s="3">
-        <v>9.9740935758266518E-3</v>
+        <v>5.1854061251645238E-3</v>
       </c>
       <c r="J12" s="3">
-        <v>7.5053475397148899E-3</v>
+        <v>6.2824006476289943E-3</v>
       </c>
       <c r="K12" s="3">
-        <v>9.3815353430275871E-3</v>
+        <v>6.7732425913520026E-3</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:L12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5317EF6B-5B69-4FC9-A4C0-27E0A6079B57}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>500000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>50000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4">
+        <v>10000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55838E95-87B8-4785-BD8F-7353E52C3BF4}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="61" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="18">
+        <v>8</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="18">
+        <v>100</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="18">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0.21</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.18</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0.23</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>0.2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>15000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
+        <v>20000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>30000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23">
+        <v>50000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24">
+        <v>12000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25">
+        <v>4200</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26">
+        <v>12000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27">
+        <v>7000</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26D7A86-4E3D-4BFB-8963-209936CC239B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC98696-EDA2-432B-B53D-0A9731CD9D3B}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4">
+        <v>1.2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5">
+        <v>1.05</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6">
+        <v>1.3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>1.3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8">
+        <v>1.4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9">
+        <v>1.7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11">
+        <v>1.3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12">
+        <v>0.7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14">
+        <v>0.8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15">
+        <v>0.6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16">
+        <v>0.4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17">
+        <v>0.6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18">
+        <v>0.7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19">
+        <v>0.8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20">
+        <v>0.3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21">
+        <v>0.4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3077B532-CB5C-4299-BC01-C4CEE62D03FA}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2">
+        <f ca="1">ROUND(RAND(),0)</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:K2" ca="1" si="0">ROUND(RAND(),0)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:K11" ca="1" si="1">ROUND(RAND(),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B2:K11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1993,495 +3514,76 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5317EF6B-5B69-4FC9-A4C0-27E0A6079B57}">
-  <dimension ref="A1:C3"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46399FE8-C706-44FC-BBC6-1A0A3571D412}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="B2">
-        <v>500000</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="B3">
-        <v>50000</v>
+        <v>0.05</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55838E95-87B8-4785-BD8F-7353E52C3BF4}">
-  <dimension ref="A1:G38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="61" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="18">
-        <v>8</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="18">
-        <v>100</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="18">
-        <v>2000</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="18">
-        <v>0.8</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="18">
-        <v>0.2</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="18">
-        <v>0.2</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="18">
-        <v>0.15</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="18">
-        <v>0.21</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="18">
-        <v>0.18</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="20"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="18">
-        <v>0.23</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18">
-        <v>0.2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20">
-        <v>15000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21">
-        <v>20000</v>
-      </c>
-      <c r="C21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22">
-        <v>30000</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23">
-        <v>50000</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24">
-        <v>12000</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25">
-        <v>4200</v>
-      </c>
-      <c r="C25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26">
-        <v>12000</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27">
-        <v>7000</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Final simulator version 1.0
</commit_message>
<xml_diff>
--- a/condiciones_iniciales/parameters.xlsx
+++ b/condiciones_iniciales/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.amador\Desktop\simulador-resiliencia\herramienta-resiliencia-simulador\condiciones_iniciales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8685B15-777C-49EB-BE9E-5D05709F6B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36F21C7-6723-405F-BB02-CC9798C6B49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transformation_rates" sheetId="1" r:id="rId1"/>
@@ -2054,7 +2054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55838E95-87B8-4785-BD8F-7353E52C3BF4}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -2916,7 +2916,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3623,7 +3623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0384CE63-9174-4422-8517-BE7A38954B2F}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Transformation time series added
</commit_message>
<xml_diff>
--- a/condiciones_iniciales/parameters.xlsx
+++ b/condiciones_iniciales/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.amador\Desktop\simulador-resiliencia\herramienta-resiliencia-simulador\condiciones_iniciales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA5215B-0045-41D4-B0FC-B408321124CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35664804-EE1F-4A85-925C-EBA67787569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transformation_rates" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="310">
   <si>
     <t>matriz</t>
   </si>
@@ -195,12 +195,6 @@
   </si>
   <si>
     <t>Tasa</t>
-  </si>
-  <si>
-    <t>Qm</t>
-  </si>
-  <si>
-    <t>Caudal medio a la salida de la región de estudio</t>
   </si>
   <si>
     <t>ConsIndusEner</t>
@@ -1007,7 +1001,19 @@
     <t>Peso del cuidado del bosque</t>
   </si>
   <si>
-    <t>Factor de incremento de conflictos socioambientales - número de solicitudes, PQRs</t>
+    <t>Número de solicitudes, PQRs</t>
+  </si>
+  <si>
+    <t>OHTS</t>
+  </si>
+  <si>
+    <t>Oferta hídrica total superficial</t>
+  </si>
+  <si>
+    <t>OHTD</t>
+  </si>
+  <si>
+    <t>Oferta hídrica total disponible</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1640,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1789,15 +1795,22 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2035,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2055,10 +2068,10 @@
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="21.5703125" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="26" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2096,21 +2109,8 @@
         <v>11</v>
       </c>
       <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-    </row>
-    <row r="2" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2124,13 +2124,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="9">
-        <v>15.10363272</v>
+        <v>0</v>
       </c>
       <c r="F2" s="9">
-        <v>0.36161662300000003</v>
+        <v>0</v>
       </c>
       <c r="G2" s="9">
-        <v>1.4353949999999999E-3</v>
+        <v>3.0775399999999998E-4</v>
       </c>
       <c r="H2" s="9">
         <v>0</v>
@@ -2139,16 +2139,16 @@
         <v>0</v>
       </c>
       <c r="J2" s="9">
-        <v>0.97649778399999998</v>
+        <v>2.255192E-2</v>
       </c>
       <c r="K2" s="9">
-        <v>0.22348389499999999</v>
+        <v>1.6105932E-2</v>
       </c>
       <c r="L2" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -2186,103 +2186,103 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="12">
-        <v>0.12250675599999999</v>
+        <v>5.1544822999999997E-2</v>
       </c>
       <c r="C4" s="12">
-        <v>0.165425198</v>
+        <v>6.9602793999999996E-2</v>
       </c>
       <c r="D4" s="11">
         <v>0</v>
       </c>
       <c r="E4" s="9">
-        <v>2.8830342099999999</v>
+        <v>1.2130391250000001</v>
       </c>
       <c r="F4" s="9">
-        <v>0.20192818900000001</v>
+        <v>8.4961459000000003E-2</v>
       </c>
       <c r="G4" s="9">
-        <v>0.22504128100000001</v>
+        <v>9.4686312999999994E-2</v>
       </c>
       <c r="H4" s="9">
         <v>0</v>
       </c>
       <c r="I4" s="9">
-        <v>1.2675275999999999E-2</v>
+        <v>5.3331330000000003E-3</v>
       </c>
       <c r="J4" s="9">
-        <v>2.1399850000000002E-2</v>
+        <v>9.0040050000000007E-3</v>
       </c>
       <c r="K4" s="9">
-        <v>6.1474160000000002E-3</v>
+        <v>2.586531E-3</v>
       </c>
       <c r="L4" s="12">
-        <v>2.2411983E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+        <v>9.4298609999999995E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="13">
-        <v>0.41466324599999999</v>
+        <v>7.4738310000000002E-3</v>
       </c>
       <c r="C5" s="13">
-        <v>0.67882470900000003</v>
+        <v>1.2235039E-2</v>
       </c>
       <c r="D5" s="13">
-        <v>0.92287318699999998</v>
+        <v>1.6633734000000001E-2</v>
       </c>
       <c r="E5" s="11">
         <v>0</v>
       </c>
       <c r="F5" s="9">
-        <v>3.9141052000000003E-2</v>
+        <v>7.0547299999999997E-4</v>
       </c>
       <c r="G5" s="9">
-        <v>1.123063924</v>
-      </c>
-      <c r="H5" s="9">
-        <v>4.3820550000000002E-3</v>
+        <v>2.0241944000000001E-2</v>
+      </c>
+      <c r="H5" s="84">
+        <v>7.8999999999999996E-5</v>
       </c>
       <c r="I5" s="9">
-        <v>6.9719847000000001E-2</v>
+        <v>1.2566210000000001E-3</v>
       </c>
       <c r="J5" s="9">
-        <v>0.29438345799999999</v>
-      </c>
-      <c r="K5" s="9">
-        <v>5.4793960000000001E-3</v>
+        <v>5.3059250000000004E-3</v>
+      </c>
+      <c r="K5" s="84">
+        <v>9.8800000000000003E-5</v>
       </c>
       <c r="L5" s="13">
-        <v>0.219559225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3.957304E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="12">
-        <v>2.5525147000000002E-2</v>
-      </c>
-      <c r="C6" s="12">
-        <v>4.3547009999999999E-3</v>
+        <v>1.90084E-4</v>
+      </c>
+      <c r="C6" s="85">
+        <v>3.2400000000000001E-5</v>
       </c>
       <c r="D6" s="9">
-        <v>8.4028898779999999</v>
+        <v>6.2575680999999994E-2</v>
       </c>
       <c r="E6" s="9">
-        <v>0.57065107599999998</v>
+        <v>4.2495950000000001E-3</v>
       </c>
       <c r="F6" s="11">
         <v>0</v>
       </c>
-      <c r="G6" s="9">
-        <v>7.2741480000000002E-3</v>
+      <c r="G6" s="84">
+        <v>5.4200000000000003E-5</v>
       </c>
       <c r="H6" s="9">
         <v>0</v>
@@ -2294,30 +2294,30 @@
         <v>0</v>
       </c>
       <c r="K6" s="9">
-        <v>7.5304041000000002E-2</v>
+        <v>5.6078300000000003E-4</v>
       </c>
       <c r="L6" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="13">
-        <v>0.41042035300000002</v>
+        <v>6.8515449999999997E-3</v>
       </c>
       <c r="C7" s="13">
-        <v>1.612068794</v>
+        <v>6.5704184999999998E-2</v>
       </c>
       <c r="D7" s="9">
-        <v>0.25722502899999999</v>
+        <v>0</v>
       </c>
       <c r="E7" s="9">
-        <v>7.8528770699999999</v>
+        <v>0</v>
       </c>
       <c r="F7" s="9">
-        <v>0.20690913799999999</v>
+        <v>0</v>
       </c>
       <c r="G7" s="11">
         <v>0</v>
@@ -2329,36 +2329,36 @@
         <v>0</v>
       </c>
       <c r="J7" s="9">
-        <v>0.81161112899999999</v>
+        <v>1.8743913000000001E-2</v>
       </c>
       <c r="K7" s="9">
         <v>0</v>
       </c>
       <c r="L7" s="12">
-        <v>5.3537469999999998E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+        <v>2.3522959999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="13">
-        <v>0.33295302100000002</v>
+        <v>0</v>
       </c>
       <c r="C8" s="13">
-        <v>2.7237237400000001</v>
+        <v>0</v>
       </c>
       <c r="D8" s="9">
-        <v>0.76523078499999997</v>
+        <v>0</v>
       </c>
       <c r="E8" s="9">
-        <v>2.4961753280000001</v>
+        <v>0</v>
       </c>
       <c r="F8" s="9">
         <v>0</v>
       </c>
       <c r="G8" s="9">
-        <v>10.3485844</v>
+        <v>0</v>
       </c>
       <c r="H8" s="11">
         <v>0</v>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -2387,10 +2387,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="9">
-        <v>0.37748686799999998</v>
+        <v>0</v>
       </c>
       <c r="E9" s="9">
-        <v>3.655071247</v>
+        <v>0</v>
       </c>
       <c r="F9" s="9">
         <v>0</v>
@@ -2414,21 +2414,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="13">
-        <v>0.71703737000000001</v>
+        <v>1.1970201E-2</v>
       </c>
       <c r="C10" s="12">
-        <v>6.8920968999999999E-2</v>
+        <v>2.809059E-3</v>
       </c>
       <c r="D10" s="9">
-        <v>1.3342369140000001</v>
+        <v>0</v>
       </c>
       <c r="E10" s="9">
-        <v>2.7573941780000002</v>
+        <v>0</v>
       </c>
       <c r="F10" s="9">
         <v>0</v>
@@ -2440,48 +2440,48 @@
         <v>0</v>
       </c>
       <c r="I10" s="9">
-        <v>9.7267363949999996</v>
+        <v>4.992328E-2</v>
       </c>
       <c r="J10" s="11">
         <v>0</v>
       </c>
       <c r="K10" s="9">
-        <v>0.18922773200000001</v>
+        <v>1.3637175E-2</v>
       </c>
       <c r="L10" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="13">
-        <v>2.9918330869999998</v>
+        <v>4.9945574E-2</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
       </c>
       <c r="D11" s="9">
-        <v>1.1734580000000001E-3</v>
+        <v>7.9209415000000005E-2</v>
       </c>
       <c r="E11" s="9">
-        <v>9.1461999999999999E-4</v>
+        <v>1.21728872</v>
       </c>
       <c r="F11" s="9">
-        <v>1.4983119999999999E-3</v>
+        <v>8.5666932000000001E-2</v>
       </c>
       <c r="G11" s="9">
-        <v>1.316025E-3</v>
-      </c>
-      <c r="H11" s="9">
-        <v>1.5161479999999999E-3</v>
-      </c>
-      <c r="I11" s="9">
-        <v>1.5833209999999999E-3</v>
-      </c>
-      <c r="J11" s="9">
-        <v>1.523106E-3</v>
+        <v>2.8216100000000001E-4</v>
+      </c>
+      <c r="H11" s="84">
+        <v>7.8999999999999996E-5</v>
+      </c>
+      <c r="I11" s="84">
+        <v>8.1300000000000001E-6</v>
+      </c>
+      <c r="J11" s="84">
+        <v>3.5200000000000002E-5</v>
       </c>
       <c r="K11" s="11">
         <v>0</v>
@@ -2490,33 +2490,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="9">
-        <v>3.8731839999999997E-2</v>
+        <v>6.4658800000000002E-4</v>
       </c>
       <c r="C12" s="13">
-        <v>0.53023689100000004</v>
+        <v>2.1611226000000001E-2</v>
       </c>
       <c r="D12" s="13">
-        <v>10.824339139999999</v>
+        <v>0</v>
       </c>
       <c r="E12" s="16">
-        <v>2.1800107230000001</v>
+        <v>0</v>
       </c>
       <c r="F12" s="12">
-        <v>3.8595233999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="16">
-        <v>0.57041623600000002</v>
+        <v>0.12229936499999999</v>
       </c>
       <c r="H12" s="14">
         <v>0</v>
       </c>
-      <c r="I12" s="12">
-        <v>1.1140082000000001E-2</v>
+      <c r="I12" s="85">
+        <v>5.7200000000000001E-5</v>
       </c>
       <c r="J12" s="12">
         <v>0</v>
@@ -2528,16 +2528,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5507,7 +5507,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5516,7 +5516,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5542,134 +5542,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="B2" s="75">
+        <v>235</v>
+      </c>
+      <c r="B2" s="74">
         <v>31</v>
       </c>
-      <c r="C2" s="74" t="s">
-        <v>307</v>
+      <c r="C2" s="82" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B3" s="21">
         <v>0.5</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B4" s="21">
         <v>0.5</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B5" s="21">
         <v>0.25</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B6" s="36">
         <v>26</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B7" s="36">
         <v>0.3380199179847686</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B8" s="36">
         <v>0.3380199179847686</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B9" s="21">
         <v>0.8</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B10" s="21">
         <v>0.5</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B11" s="21">
         <v>0.3</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B12" s="21">
         <v>0.1</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B13" s="21">
         <v>1</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6680,22 +6680,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="E1" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="F1" s="38" t="s">
         <v>262</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>264</v>
       </c>
       <c r="G1" s="39" t="s">
         <v>14</v>
@@ -6703,22 +6703,22 @@
     </row>
     <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="41" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="D2" s="41" t="s">
         <v>266</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="E2" s="42" t="s">
         <v>267</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="F2" s="42" t="s">
         <v>268</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>269</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>270</v>
       </c>
       <c r="G2" s="43">
         <v>0</v>
@@ -6726,22 +6726,22 @@
     </row>
     <row r="3" spans="1:7" ht="84.75" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>271</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="D3" s="46" t="s">
         <v>272</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="E3" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="F3" s="48" t="s">
         <v>273</v>
-      </c>
-      <c r="D3" s="46" t="s">
-        <v>274</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>269</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>275</v>
       </c>
       <c r="G3" s="43">
         <v>0.63780000000000003</v>
@@ -6749,116 +6749,116 @@
     </row>
     <row r="4" spans="1:7" ht="37.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>271</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="D4" s="50" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>273</v>
-      </c>
-      <c r="D4" s="50" t="s">
+      <c r="F4" s="51" t="s">
         <v>277</v>
       </c>
-      <c r="E4" s="50" t="s">
-        <v>278</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>279</v>
-      </c>
-      <c r="G4" s="78">
+      <c r="G4" s="77">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="53" t="s">
         <v>280</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="D5" s="54" t="s">
         <v>281</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="E5" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="F5" s="55" t="s">
         <v>283</v>
       </c>
-      <c r="E5" s="47" t="s">
-        <v>284</v>
-      </c>
-      <c r="F5" s="55" t="s">
-        <v>285</v>
-      </c>
-      <c r="G5" s="79">
-        <v>27</v>
+      <c r="G5" s="78">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B6" s="57" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" s="59" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="E6" s="60" t="s">
+        <v>282</v>
+      </c>
+      <c r="F6" s="61" t="s">
         <v>287</v>
       </c>
-      <c r="D6" s="59" t="s">
-        <v>288</v>
-      </c>
-      <c r="E6" s="60" t="s">
-        <v>284</v>
-      </c>
-      <c r="F6" s="61" t="s">
-        <v>289</v>
-      </c>
-      <c r="G6" s="80">
+      <c r="G6" s="79">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C7" s="58" t="s">
+        <v>285</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="E7" s="60" t="s">
+        <v>282</v>
+      </c>
+      <c r="F7" s="61" t="s">
         <v>287</v>
       </c>
-      <c r="D7" s="59" t="s">
-        <v>288</v>
-      </c>
-      <c r="E7" s="60" t="s">
-        <v>284</v>
-      </c>
-      <c r="F7" s="61" t="s">
-        <v>289</v>
-      </c>
-      <c r="G7" s="80">
+      <c r="G7" s="79">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="62" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C8" s="64" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>286</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>282</v>
+      </c>
+      <c r="F8" s="67" t="s">
         <v>287</v>
       </c>
-      <c r="D8" s="65" t="s">
-        <v>288</v>
-      </c>
-      <c r="E8" s="66" t="s">
-        <v>284</v>
-      </c>
-      <c r="F8" s="67" t="s">
-        <v>289</v>
-      </c>
-      <c r="G8" s="81">
+      <c r="G8" s="80">
         <v>3</v>
       </c>
     </row>
@@ -7877,13 +7877,13 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B2" s="72">
         <v>10</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -7911,46 +7911,46 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B3" s="73">
         <v>10</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B4" s="71">
         <v>10000</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B5" s="71">
         <v>6929</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B6" s="24">
         <v>0.51800000000000002</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8943,7 +8943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -9084,7 +9084,7 @@
         <v>2040</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10075,10 +10075,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:J999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10107,7 +10107,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="26">
-        <v>5000000</v>
+        <v>10000000</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>39</v>
@@ -10119,7 +10119,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="26">
-        <v>10000000</v>
+        <v>20000000</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>41</v>
@@ -10131,7 +10131,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="26">
-        <v>20000000</v>
+        <v>25</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>43</v>
@@ -10143,7 +10143,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="26">
-        <v>25</v>
+        <v>0.8</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>45</v>
@@ -10155,19 +10155,20 @@
         <v>46</v>
       </c>
       <c r="B6" s="26">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="26"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="26">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>49</v>
@@ -10179,59 +10180,59 @@
       <c r="A8" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="26">
-        <v>0.2</v>
+      <c r="B8" s="72">
+        <v>0.31</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="26"/>
-      <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="72">
-        <v>0.31</v>
+        <v>0.13</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>53</v>
       </c>
       <c r="G9" s="26"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="72">
-        <v>0.13</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>55</v>
       </c>
+      <c r="E10" s="17"/>
       <c r="G10" s="26"/>
-      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="72">
-        <v>0.46600000000000003</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="17"/>
       <c r="G11" s="26"/>
+      <c r="J11" s="26"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="72">
-        <v>0.57999999999999996</v>
+      <c r="B12" s="75">
+        <v>280</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>59</v>
@@ -10240,17 +10241,16 @@
       <c r="J12" s="26"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="76">
-        <v>280</v>
-      </c>
-      <c r="C13" s="26" t="s">
+      <c r="B13" s="21">
+        <v>75</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="J13" s="26"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
@@ -10268,13 +10268,14 @@
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="21">
-        <v>75</v>
+      <c r="B15" s="73">
+        <v>60.817417589999998</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>65</v>
       </c>
       <c r="G15" s="27"/>
+      <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
@@ -10289,100 +10290,108 @@
       <c r="G16" s="27"/>
       <c r="J16" s="26"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="73">
-        <v>60.817417589999998</v>
+      <c r="B17" s="21">
+        <v>80</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>69</v>
       </c>
       <c r="G17" s="27"/>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="21">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>71</v>
       </c>
       <c r="G18" s="27"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>72</v>
       </c>
       <c r="B19" s="21">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>73</v>
       </c>
       <c r="G19" s="27"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="21">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>75</v>
       </c>
       <c r="G20" s="27"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="21">
-        <v>40</v>
-      </c>
-      <c r="C21" s="21" t="s">
+        <v>0.6</v>
+      </c>
+      <c r="C21" s="76" t="s">
         <v>77</v>
       </c>
       <c r="G21" s="27"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>78</v>
       </c>
       <c r="B22" s="21">
-        <v>0.6</v>
-      </c>
-      <c r="C22" s="77" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>79</v>
       </c>
       <c r="G22" s="27"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="21">
-        <v>600</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>306</v>
+      </c>
+      <c r="B23" s="26">
+        <v>200000000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>308</v>
+      </c>
+      <c r="B24" s="26">
+        <v>105000000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11350,7 +11359,6 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11377,19 +11385,19 @@
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="28"/>
       <c r="B1" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>86</v>
       </c>
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
@@ -11414,7 +11422,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" s="21">
         <v>0.5</v>
@@ -11434,7 +11442,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="21">
         <v>0.5</v>
@@ -11454,7 +11462,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" s="21">
         <v>0.3</v>
@@ -11474,7 +11482,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="21">
         <v>0.4</v>
@@ -11494,7 +11502,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="21">
         <v>0.6</v>
@@ -11514,7 +11522,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="21">
         <v>0.7</v>
@@ -11534,7 +11542,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="21">
         <v>0.8</v>
@@ -11554,7 +11562,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="21">
         <v>0.6</v>
@@ -11574,7 +11582,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10" s="21">
         <v>0.7</v>
@@ -11594,7 +11602,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" s="21">
         <v>0.8</v>
@@ -14590,7 +14598,7 @@
   <dimension ref="A1:G991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B10" sqref="B10:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14606,27 +14614,27 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
       <c r="B1" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>100</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="29">
         <v>35.799999999999997</v>
@@ -14649,7 +14657,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="29">
         <v>34.46</v>
@@ -14670,7 +14678,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="29">
         <v>36.4</v>
@@ -14681,7 +14689,7 @@
       <c r="D4" s="29">
         <v>6.3</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="83">
         <v>616.51</v>
       </c>
       <c r="F4" s="27"/>
@@ -14691,7 +14699,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" s="29">
         <v>34.79</v>
@@ -14712,7 +14720,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="29">
         <v>36.03</v>
@@ -14733,7 +14741,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" s="29">
         <v>37.950000000000003</v>
@@ -14754,7 +14762,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" s="29">
         <v>35.39</v>
@@ -14775,7 +14783,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B9" s="29">
         <v>34.82</v>
@@ -14796,7 +14804,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B10" s="29">
         <v>122.28</v>
@@ -14817,7 +14825,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" s="29">
         <v>129.30000000000001</v>
@@ -14838,7 +14846,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B12" s="29">
         <v>116.63</v>
@@ -14861,7 +14869,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B13" s="29">
         <v>132.80000000000001</v>
@@ -14882,7 +14890,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="29">
         <v>112.6</v>
@@ -14903,7 +14911,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B15" s="29">
         <v>163.72</v>
@@ -14924,7 +14932,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B16" s="29">
         <v>126.21</v>
@@ -14945,7 +14953,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B17" s="29">
         <v>70.430000000000007</v>
@@ -14966,7 +14974,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B18" s="29">
         <v>33.61</v>
@@ -14987,7 +14995,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B19" s="29">
         <v>33.1</v>
@@ -15008,7 +15016,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B20" s="29">
         <v>35.78</v>
@@ -15031,7 +15039,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B21" s="29">
         <v>35.46</v>
@@ -15052,7 +15060,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B22" s="29">
         <v>33.26</v>
@@ -15073,7 +15081,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B23" s="29">
         <v>32.39</v>
@@ -15094,7 +15102,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B24" s="29">
         <v>33.119999999999997</v>
@@ -15115,7 +15123,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B25" s="29">
         <v>153.5</v>
@@ -15136,7 +15144,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B26" s="29">
         <v>135.12</v>
@@ -15157,7 +15165,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" s="29">
         <v>100.99</v>
@@ -15176,7 +15184,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B28" s="29">
         <v>72.64</v>
@@ -15197,7 +15205,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B29" s="29">
         <v>110.44</v>
@@ -15218,7 +15226,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B30" s="29">
         <v>38.479999999999997</v>
@@ -16217,7 +16225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -16234,27 +16242,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2" s="26">
         <v>55</v>
@@ -16274,7 +16282,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" s="26">
         <v>55</v>
@@ -16294,7 +16302,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B4" s="26">
         <v>55</v>
@@ -16314,7 +16322,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B5" s="26">
         <v>55</v>
@@ -16334,7 +16342,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6" s="26">
         <v>55</v>
@@ -16354,7 +16362,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B7" s="26">
         <v>55</v>
@@ -16374,7 +16382,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" s="26">
         <v>70</v>
@@ -16394,7 +16402,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B9" s="26">
         <v>80</v>
@@ -16414,7 +16422,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B10" s="26">
         <v>55</v>
@@ -16434,7 +16442,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B11" s="26">
         <v>55</v>
@@ -17443,7 +17451,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17467,46 +17475,46 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B2" s="31">
         <v>1.04E-2</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B3" s="31">
         <v>8.7300000000000003E-2</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" s="31">
         <v>2012</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" s="31">
         <v>2018</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -18506,7 +18514,7 @@
   <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18523,27 +18531,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>157</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B2" s="21">
         <v>1</v>
@@ -18566,7 +18574,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="21">
         <v>1</v>
@@ -18589,7 +18597,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" s="21">
         <v>1</v>
@@ -18612,7 +18620,7 @@
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -18635,7 +18643,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B6" s="21">
         <v>1</v>
@@ -18658,7 +18666,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B7" s="21">
         <v>1</v>
@@ -18681,7 +18689,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B8" s="21">
         <v>0</v>
@@ -18704,7 +18712,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B9" s="21">
         <v>1</v>
@@ -19725,8 +19733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19754,408 +19762,408 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B2" s="32">
         <v>1.9609999999999999E-2</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" s="32">
         <v>1.4293000000000001E-3</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" s="32">
         <v>2.34E-5</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B5" s="32">
         <v>2.2599999999999999E-3</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B6" s="32">
         <v>6.9300000000000004E-3</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B7" s="32">
         <v>4.1079999999999998E-2</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B8" s="26">
         <v>27</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B9" s="26">
         <v>35</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B10" s="26">
         <v>3</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B11" s="26">
         <v>22</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B12" s="26">
         <v>28</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" s="26">
         <v>2</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="B14" s="76">
-        <v>2.5204</v>
+        <v>189</v>
+      </c>
+      <c r="B14" s="75">
+        <v>1.779E-2</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B15" s="76">
-        <v>5</v>
+        <v>191</v>
+      </c>
+      <c r="B15" s="75">
+        <v>2.1270000000000001E-2</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="B16" s="76">
-        <v>4.0800000000000003E-2</v>
+        <v>193</v>
+      </c>
+      <c r="B16" s="75">
+        <v>1.3799999999999999E-3</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="B17" s="76">
-        <v>1.2438579220000001E-2</v>
+        <v>195</v>
+      </c>
+      <c r="B17" s="75">
+        <v>6.4159999999999995E-2</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="B18" s="82">
+        <v>197</v>
+      </c>
+      <c r="B18" s="81">
         <v>67</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F18" s="26"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="B19" s="82">
+        <v>199</v>
+      </c>
+      <c r="B19" s="81">
         <v>41</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F19" s="26"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="B20" s="82">
+        <v>201</v>
+      </c>
+      <c r="B20" s="81">
         <v>8</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F20" s="26"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" s="82">
+        <v>203</v>
+      </c>
+      <c r="B21" s="81">
         <v>27</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F21" s="26"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="B22" s="82">
+        <v>205</v>
+      </c>
+      <c r="B22" s="81">
         <v>29</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F22" s="26"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="B23" s="82">
+        <v>207</v>
+      </c>
+      <c r="B23" s="81">
         <v>87</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F23" s="26"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="B24" s="82">
+        <v>209</v>
+      </c>
+      <c r="B24" s="81">
         <v>34</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F24" s="26"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="B25" s="82">
+        <v>211</v>
+      </c>
+      <c r="B25" s="81">
         <v>22</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="B26" s="82">
+        <v>213</v>
+      </c>
+      <c r="B26" s="81">
         <v>6</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F26" s="26"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
-        <v>217</v>
-      </c>
-      <c r="B27" s="82">
+        <v>215</v>
+      </c>
+      <c r="B27" s="81">
         <v>4</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F27" s="26"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="B28" s="82">
+        <v>217</v>
+      </c>
+      <c r="B28" s="81">
         <v>4</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F28" s="26"/>
       <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="B29" s="82">
+        <v>219</v>
+      </c>
+      <c r="B29" s="81">
         <v>21</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F29" s="26"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B30" s="26">
         <v>43</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F30" s="26"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B31" s="26">
         <v>32</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="26"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B32" s="26">
         <v>0.79700000000000004</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F32" s="26"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B33" s="26">
         <v>0.17249999999999999</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B34" s="26">
         <v>6.4799999999999996E-2</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B35" s="26">
         <v>1</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B36" s="26">
         <v>1</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
udated the weights to the resilience indicator
</commit_message>
<xml_diff>
--- a/condiciones_iniciales/parameters.xlsx
+++ b/condiciones_iniciales/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.amador\Desktop\simulador-resiliencia\herramienta-resiliencia-simulador\condiciones_iniciales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D6DB7-8DE1-4892-8F45-7094C99A2B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B77A51E-A013-495C-9C8F-0BAEBC6BAE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transformation_rates" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="393">
   <si>
     <t>matriz</t>
   </si>
@@ -1238,17 +1238,46 @@
   </si>
   <si>
     <t>Agropecuario heterogeneo'</t>
+  </si>
+  <si>
+    <t>p_transitividad</t>
+  </si>
+  <si>
+    <t>Porcentaje de transitividad</t>
+  </si>
+  <si>
+    <t>BOmax</t>
+  </si>
+  <si>
+    <t>Bosque máximo en la región de estudio</t>
+  </si>
+  <si>
+    <t>Nectarivoro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1378,8 +1407,22 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1432,6 +1475,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1862,173 +1911,180 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="22" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="23" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="24" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8072,7 +8128,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8170,6 +8226,17 @@
       </c>
       <c r="C6" s="12" t="s">
         <v>281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="85" t="s">
+        <v>388</v>
+      </c>
+      <c r="B7" s="61">
+        <v>0.8</v>
+      </c>
+      <c r="C7" s="85" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9162,7 +9229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -9278,7 +9345,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>33</v>
@@ -10297,7 +10364,7 @@
   <dimension ref="A1:J999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10325,7 +10392,7 @@
       <c r="A2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="84">
         <v>1000</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -14836,8 +14903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G991"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19107,7 +19174,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19174,9 +19241,15 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="59" t="s">
+        <v>390</v>
+      </c>
+      <c r="B6" s="87">
+        <v>17026.634300000002</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>391</v>
+      </c>
       <c r="E6" s="8"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20167,22 +20240,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G999"/>
+  <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="25" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="25" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -20193,42 +20269,48 @@
         <v>135</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>140</v>
       </c>
       <c r="B2" s="12">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0</v>
+      </c>
+      <c r="D2" s="83">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="12">
+      <c r="F2" s="12">
+        <v>0</v>
+      </c>
+      <c r="G2" s="12">
         <v>1</v>
       </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12">
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="F2" s="12">
-        <v>1</v>
-      </c>
-      <c r="G2" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>141</v>
       </c>
@@ -20236,7 +20318,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="12">
         <v>0</v>
@@ -20250,8 +20332,11 @@
       <c r="G3" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>142</v>
       </c>
@@ -20268,18 +20353,21 @@
         <v>0</v>
       </c>
       <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12">
         <v>0</v>
       </c>
-      <c r="G4" s="12">
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>282</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -20296,31 +20384,37 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>143</v>
       </c>
       <c r="B6" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="12">
         <v>0</v>
       </c>
       <c r="F6" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>144</v>
       </c>
@@ -20334,7 +20428,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="12">
         <v>0</v>
@@ -20342,19 +20436,22 @@
       <c r="G7" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>145</v>
       </c>
       <c r="B8" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="12">
         <v>0</v>
       </c>
       <c r="D8" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="12">
         <v>0</v>
@@ -20365,8 +20462,11 @@
       <c r="G8" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>146</v>
       </c>
@@ -20386,6 +20486,9 @@
         <v>0</v>
       </c>
       <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>1</v>
       </c>
     </row>
@@ -21370,18 +21473,18 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="B2:G9">
+  <conditionalFormatting sqref="B2:H9">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G9">
+  <conditionalFormatting sqref="B2:H9">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
delta time and accumulated slopes added to the output
</commit_message>
<xml_diff>
--- a/condiciones_iniciales/parameters.xlsx
+++ b/condiciones_iniciales/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.amador\Desktop\simulador-resiliencia\herramienta-resiliencia-simulador\condiciones_iniciales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B77A51E-A013-495C-9C8F-0BAEBC6BAE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7446E692-A63E-4677-B53C-AB8DE77F6C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transformation_rates" sheetId="1" r:id="rId1"/>
@@ -1259,7 +1259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1412,14 +1412,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1913,7 +1905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2079,7 +2071,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8128,7 +8119,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8229,13 +8220,13 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="84" t="s">
         <v>388</v>
       </c>
       <c r="B7" s="61">
         <v>0.8</v>
       </c>
-      <c r="C7" s="85" t="s">
+      <c r="C7" s="84" t="s">
         <v>389</v>
       </c>
     </row>
@@ -10392,7 +10383,7 @@
       <c r="A2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="84">
+      <c r="B2" s="83">
         <v>1000</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -19174,7 +19165,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19244,7 +19235,7 @@
       <c r="A6" s="59" t="s">
         <v>390</v>
       </c>
-      <c r="B6" s="87">
+      <c r="B6" s="86">
         <v>17026.634300000002</v>
       </c>
       <c r="C6" s="59" t="s">
@@ -20243,7 +20234,7 @@
   <dimension ref="A1:H999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20294,7 +20285,7 @@
       <c r="C2" s="12">
         <v>0</v>
       </c>
-      <c r="D2" s="83">
+      <c r="D2" s="85">
         <v>0</v>
       </c>
       <c r="E2" s="12">
@@ -20384,7 +20375,7 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="86">
+      <c r="H5" s="85">
         <v>1</v>
       </c>
     </row>

</xml_diff>